<commit_message>
Arrhythmia anomaly scores fixed and metrics recalculated
</commit_message>
<xml_diff>
--- a/metrics/AUC.xlsx
+++ b/metrics/AUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0132030\Desktop\First paper\EJOR\repo\benchmarking-anomaly-detection\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAC2BB17-8DF4-4D99-97DE-9DA35C554D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F14F9E1-022D-4443-8E76-B2E2F400495C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6AB05D4E-90B6-43B6-8049-5D74BC798D35}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3">
-        <v>0.20717538075050976</v>
+        <v>0.79311247186894829</v>
       </c>
       <c r="C2" s="3">
         <v>0.72020725388601037</v>

</xml_diff>